<commit_message>
File Reader for hospital and Intensive Care, added Critital stage
</commit_message>
<xml_diff>
--- a/PopulationBySwedishRegion.xlsx
+++ b/PopulationBySwedishRegion.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/Documents/corona/SEQJIR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5DEC4D-2986-A947-94BD-112BC972C285}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C641F32-F2F9-B54C-9F17-5821B8347165}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="1120" windowWidth="27640" windowHeight="16540" xr2:uid="{894A8C14-C469-7947-B8BB-D8E5FAE1679C}"/>
+    <workbookView xWindow="1160" yWindow="620" windowWidth="27640" windowHeight="16540" xr2:uid="{894A8C14-C469-7947-B8BB-D8E5FAE1679C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Blekinge</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Östergötland</t>
+  </si>
+  <si>
+    <t>Sverige</t>
   </si>
 </sst>
 </file>
@@ -137,9 +140,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAE9617B-9A63-9F47-89B1-4E36A756A529}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,6 +638,14 @@
         <v>465495</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>10300000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>